<commit_message>
02/01/2023 v.0.0.2 - Se añaden las columnas "Tipo de administración", "Código Postal", "Descripción de la financiación europea" y "Directiva de aplicación"
</commit_message>
<xml_diff>
--- a/dist/resources/base/datosAbiertos-PLACSP.xlsx
+++ b/dist/resources/base/datosAbiertos-PLACSP.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Resultados" r:id="rId6" sheetId="3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Licitaciones!$A$1:$AB$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Licitaciones!$A$1:$AF$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="true">Resultados!$A$1:$Y$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -93,7 +93,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="#,##0.00 "/>
   </numFmts>
-  <fonts count="54" x14ac:knownFonts="1">
+  <fonts count="55" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +139,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -576,7 +581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="304">
+  <cellXfs count="310">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1005,6 +1010,14 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true">
       <alignment wrapText="true"/>
     </xf>
   </cellXfs>
@@ -1509,9 +1522,13 @@
     <col min="26" max="26" width="18.0" customWidth="true"/>
     <col min="27" max="27" width="18.0" customWidth="true"/>
     <col min="28" max="28" width="18.0" customWidth="true"/>
+    <col min="29" max="29" width="18.0" customWidth="true"/>
+    <col min="30" max="30" width="18.0" customWidth="true"/>
+    <col min="31" max="31" width="18.0" customWidth="true"/>
+    <col min="32" max="32" width="18.0" customWidth="true"/>
   </cols>
   <sheetData/>
-  <autoFilter ref="A1:AB1"/>
+  <autoFilter ref="A1:AF1"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>

</xml_diff>